<commit_message>
Cell formatting in tools_summary.xlsx
</commit_message>
<xml_diff>
--- a/tools_summary.xlsx
+++ b/tools_summary.xlsx
@@ -180,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -217,6 +217,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Serif"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Serif"/>
       <family val="1"/>
@@ -321,7 +328,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,6 +361,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,7 +373,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -370,7 +381,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,8 +412,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -410,9 +421,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="38.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -449,28 +460,28 @@
       <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="117.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -484,15 +495,15 @@
       <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="43.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="62.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
@@ -500,51 +511,51 @@
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="114.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update HoverNet and stain separation descriptions
</commit_message>
<xml_diff>
--- a/tools_summary.xlsx
+++ b/tools_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t xml:space="preserve">Task to achieve</t>
   </si>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">https://github.com/CBICA/HistoReg</t>
   </si>
   <si>
-    <t xml:space="preserve">I encountered some difficulties building ITK as described in installation instructions. Issues were resolved on Ubuntu 20.04 with local installation of ITK 4.13.2 using  apt package </t>
+    <t xml:space="preserve">I encountered some difficulties building ITK as described in installation instructions. Issues were resolved on Ubuntu 20.04 with local installation of ITK 4.13.2 using  apt package. </t>
   </si>
   <si>
     <t xml:space="preserve">ANHIR_MW</t>
@@ -125,6 +125,9 @@
     <t xml:space="preserve">https://github.com/vqdang/hover_net</t>
   </si>
   <si>
+    <t xml:space="preserve">Empirically, appears to be a good middle ground between StarDist and CellPose in that segmentations are not confined to star-convex polygons (StarDist) but do not overshoot the nucleus (CellPose).</t>
+  </si>
+  <si>
     <t xml:space="preserve">StarDist</t>
   </si>
   <si>
@@ -137,7 +140,7 @@
     <t xml:space="preserve">https://github.com/stardist/stardist</t>
   </si>
   <si>
-    <t xml:space="preserve">All detected objects will take rounded, star-convex polygon structure</t>
+    <t xml:space="preserve">All detected objects will take rounded, star-convex polygon structure. Tool is therefore valid on rounded nuclei but not so much on other objects that may take elongated or ‘sharp’ shapes.</t>
   </si>
   <si>
     <t xml:space="preserve">CellPose</t>
@@ -252,7 +255,7 @@
     <t xml:space="preserve">https://github.com/Peter554/StainTools/tree/master/staintools/stain_extraction</t>
   </si>
   <si>
-    <t xml:space="preserve">Separate into two stains – i.e. H&amp;E into H and E or H-DAB into H and DAB</t>
+    <t xml:space="preserve">Separation into two stains i.e. H&amp;E into H and E or H-DAB into H and DAB.</t>
   </si>
   <si>
     <t xml:space="preserve">Geijs et al., 2018</t>
@@ -264,7 +267,32 @@
     <t xml:space="preserve">https://github.com/VolodymyrChapman/AutomaticColorUnmixing_VC_branch</t>
   </si>
   <si>
-    <t xml:space="preserve">Separation into H, DAB and E (residual); GitHub repo is a public fork of an internal one developed by Geijs et al. Repo editing to increase dependency on openly accessible, stable libraries (scikit-image etc.) ongoing – contributions welcome</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Serif"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Separation into three stains i.e. H, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Serif"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">E (residual) and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Serif"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> DAB; GitHub repo is a public fork of an internal one developed by Geijs et al. Repo editing to increase dependency on openly accessible, stable libraries (scikit-image etc.) ongoing – contributions welcome</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Ruifrok &amp; Johnston, 2001</t>
@@ -276,7 +304,7 @@
     <t xml:space="preserve">https://scikit-image.org/docs/stable/api/skimage.color.html#skimage.color.rgb2hed</t>
   </si>
   <si>
-    <t xml:space="preserve">Separation into H, E and DAB</t>
+    <t xml:space="preserve">Separation into three stains i.e. H, E (residual) and DAB.</t>
   </si>
 </sst>
 </file>
@@ -286,7 +314,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -335,6 +363,11 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Serif"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -584,8 +617,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -593,7 +626,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.4"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.52"/>
@@ -657,7 +690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="72.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="122.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -673,150 +706,152 @@
       <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="62.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F4" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="103.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="100.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="72.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="72.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16"/>
       <c r="B8" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16"/>
       <c r="B9" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="106" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="128" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
edit image parsing tools
</commit_message>
<xml_diff>
--- a/tools_summary.xlsx
+++ b/tools_summary.xlsx
@@ -732,8 +732,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="B11:F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -742,7 +742,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="42.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="57.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.52"/>
   </cols>
@@ -989,7 +989,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="43.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="65.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="10" t="s">
         <v>68</v>

</xml_diff>